<commit_message>
Add improved Excel file
</commit_message>
<xml_diff>
--- a/CDPR_Revenue_Analysis.xlsx
+++ b/CDPR_Revenue_Analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tosie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tosie\Desktop\projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A8D646-3574-4CB0-A66E-D2CBBEE0BBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9695D8-8552-4811-AFEA-6CB8ACC7CC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1110" windowWidth="29040" windowHeight="17520" xr2:uid="{8D18EEC2-743B-47E3-8CD0-9B3567279D3C}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>Rok</t>
   </si>
@@ -264,9 +264,6 @@
     <t>01.07.2014-30.09.2014</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>01.10.2014-30.12.2014</t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>Prognoza spekulacyjna (z wyjątkiem Q1 2025) na podstawie danych historycznych z 2023-2025. Uwzględniono średni wzrost sezonowy (Q4 +20%). Scenariusz z dodatkiem zakłada wzrost o 263% w Q2 2026 (na podstawie efektu Phantom Liberty).</t>
+  </si>
+  <si>
+    <t>Prognoza z DLC</t>
   </si>
 </sst>
 </file>
@@ -337,7 +337,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\+0.0%;\-0.0%;0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +404,15 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -524,7 +533,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -550,21 +559,14 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -575,13 +577,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -592,13 +589,16 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +628,15 @@
     <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -637,23 +646,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -780,7 +792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88A21F28-1276-4C1B-9D42-7145C3F59A8B}" type="CELLRANGE">
+                    <a:fld id="{FFA52733-78C7-4C87-BE96-2903797ABA1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -813,7 +825,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{469F6C70-6133-4AF0-9D2B-CF3A6CE3C01D}" type="CELLRANGE">
+                    <a:fld id="{CDAA1080-DFB3-45F7-B06C-BFFECFC2B39D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -857,7 +869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9186EC43-AC61-4F00-A4AA-196BB27FB338}" type="CELLRANGE">
+                    <a:fld id="{106F4277-F7E2-48EB-8E48-B58D402E9713}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -921,7 +933,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8DE3F31E-DEBD-4499-9027-2D171C261B4E}" type="CELLRANGE">
+                    <a:fld id="{7E253321-6AAC-4435-96D8-E77E9D707F8D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -955,7 +967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFFE3F97-EA8D-475C-93CB-B2F2CB476B2E}" type="CELLRANGE">
+                    <a:fld id="{A08B42C3-E151-4E94-BB41-3A174D5BD99F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -989,7 +1001,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AF775B0-6C5B-4549-B75D-40EF0C3685E9}" type="CELLRANGE">
+                    <a:fld id="{F38B6346-34DE-4AB1-9F27-A7F5316233F7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1033,7 +1045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8AB2079A-3E49-4B64-9D19-25D78DCA30A9}" type="CELLRANGE">
+                    <a:fld id="{922AB1DD-B378-4E27-BF51-B0151C7D36AD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1067,7 +1079,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB0F819D-6C18-4EEE-989A-FA74A7903050}" type="CELLRANGE">
+                    <a:fld id="{AECE8C09-C2EF-432B-8989-7DD7EB1A5A4F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1101,7 +1113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8BA40F94-AF0F-46AB-8C29-3209DE5D4E4B}" type="CELLRANGE">
+                    <a:fld id="{28B84DC3-5351-46AE-9971-344B2FB1BBC3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1135,7 +1147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BD39DA5-F4DB-431D-B923-7B9265AF7649}" type="CELLRANGE">
+                    <a:fld id="{350F1807-9141-40D9-B394-D960E0BC98B8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1169,7 +1181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00433D7C-FF9C-4D59-9335-1204755A5A80}" type="CELLRANGE">
+                    <a:fld id="{3C766E92-36AA-4A64-8FEE-10ED8B0FEF67}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1736,7 +1748,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD7DE22D-9730-419A-B599-F3757F19A26F}" type="CELLRANGE">
+                    <a:fld id="{AB7F53D2-78C4-4B6F-84BF-DF1AE60B3765}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1769,7 +1781,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A39DF4AF-9B5E-487F-BB61-5FABBACA6FFE}" type="CELLRANGE">
+                    <a:fld id="{C72F2F14-5C69-46AC-9E05-10F417F12F55}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1803,7 +1815,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{836DF6EB-429D-4128-A3C0-28081B147FB7}" type="CELLRANGE">
+                    <a:fld id="{A7B9C603-CCD0-4BF9-BA04-A5DB8E182EA6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1852,7 +1864,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{EC7C1D38-D139-4954-B0FD-C486915A273C}" type="CELLRANGE">
+                    <a:fld id="{AE7DD490-C744-4ADF-B3B3-B9A779857C35}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr>
                         <a:defRPr sz="1100" b="1">
@@ -1934,7 +1946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A6D0091-EDD5-4EFE-B273-21C86F07D1B6}" type="CELLRANGE">
+                    <a:fld id="{CDD93E00-8441-494D-B5A8-77CC48854FD8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -1968,7 +1980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42E23383-179B-4BE3-8BDB-90CA75282202}" type="CELLRANGE">
+                    <a:fld id="{A48818EC-E4BB-4B60-9542-8C5A94A87AE6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2002,7 +2014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8143C291-24C8-4F3F-95BD-439BD10E5555}" type="CELLRANGE">
+                    <a:fld id="{37B38BE4-8469-4F35-95F8-F14AD739EEE3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2036,7 +2048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19C32348-BF34-4AA7-9977-F19DB7351103}" type="CELLRANGE">
+                    <a:fld id="{9F0FAC5C-8232-417B-B375-CF0012AB19CC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2070,7 +2082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D250DA97-2431-4C3D-B6CD-30C3F26D852B}" type="CELLRANGE">
+                    <a:fld id="{95983A72-0FDF-4FB3-B52B-30E53D0F8800}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2104,7 +2116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F1580A7-6337-4271-B32B-1FE97015F637}" type="CELLRANGE">
+                    <a:fld id="{05A9D5F5-CFBC-48BA-90AE-593CCCA0266D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2138,7 +2150,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA6890DD-BF87-4705-975B-3961F42A42AA}" type="CELLRANGE">
+                    <a:fld id="{21822C79-70E7-4DC0-BEF9-8BF40E8DB457}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2172,7 +2184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D31395B-0358-4D08-AC44-AFFB9681A3B0}" type="CELLRANGE">
+                    <a:fld id="{A05060E5-006D-4B28-8501-C8F9789F0B5D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[ZAKRES KOMÓREK]</a:t>
@@ -2367,43 +2379,43 @@
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>85022</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>136729</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>63667</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>175537</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>72418</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>127141</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>77710</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>121911</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>59087</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>88133</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>52217</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>56555</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>40675</c:v>
                 </c:pt>
               </c:numCache>
@@ -2511,7 +2523,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3161,7 +3173,7 @@
                   <c:v>755745.84061898128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>139845.52572243783</c:v>
+                  <c:v>139845.525722438</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>237058.82684164197</c:v>
@@ -6021,25 +6033,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35AC366-2D3E-4E52-ABAC-A0D15C43BCFC}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="18" customWidth="1"/>
-    <col min="7" max="7" width="11" style="18" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="18" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="6.42578125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="40" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="40" customWidth="1"/>
+    <col min="7" max="7" width="11" style="40" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="40" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="40" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6052,7 +6064,7 @@
       <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="15" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -6065,1278 +6077,1273 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45">
+    <row r="2" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>2014</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="3">
         <v>4801</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="29">
+        <v>21513</v>
+      </c>
+      <c r="G2" s="35"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7565</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2775</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>2014</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="36">
-        <v>21513</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="9"/>
+      <c r="D5" s="3">
+        <v>6372</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
-        <v>2014</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="9">
-        <v>7565</v>
-      </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45">
-        <v>2014</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="9">
-        <v>2775</v>
-      </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
-        <v>2014</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="9">
-        <v>6372</v>
-      </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="6" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>2015</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="8">
         <v>2857</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="41">
         <v>-0.40491564257446366</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="29">
         <v>630856</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="32">
         <v>28.324408497187747</v>
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>2015</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="3">
         <v>406248</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="41">
         <v>52.700991407799073</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="43"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="33"/>
       <c r="H7" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    <row r="8" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>2015</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="3">
         <v>85022</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="41">
         <v>29.638558558558557</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="43"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="33"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+    <row r="9" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>2015</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="C9" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="3">
         <v>136729</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="41">
         <v>20.457784055241682</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="44"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="34"/>
       <c r="H9" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+    <row r="10" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>2016</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="3">
         <v>63667</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="41">
         <v>21.284564228211412</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="29">
         <v>438763</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="32">
         <v>-0.30449579618803657</v>
       </c>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+    <row r="11" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>2016</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="3">
         <v>175537</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="41">
         <v>-0.56790679584884107</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="43"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+    <row r="12" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>2016</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="3">
         <v>72418</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="41">
         <v>-0.14824398391004681</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+    <row r="13" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>2016</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="14">
+      <c r="C13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="3">
         <v>127141</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="41">
         <v>-7.0124114123558276E-2</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="44"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+    <row r="14" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>2017</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="3">
         <v>77710</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="41">
         <v>0.22056952581400097</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="29">
         <v>346841</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="32">
         <v>-0.2095026244236638</v>
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+    <row r="15" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>2017</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="3">
         <v>121911</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="41">
         <v>-0.30549684681861944</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="43"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+    <row r="16" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>2017</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="3">
         <v>59087</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="41">
         <v>-0.18408406749703113</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="33"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+    <row r="17" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
         <v>2017</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="14">
+      <c r="C17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3">
         <v>88133</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="41">
         <v>-0.30680897586144518</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="44"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+    <row r="18" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>2018</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="3">
         <v>52217</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="41">
         <v>-0.32805301762964867</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="29">
         <v>235919</v>
       </c>
-      <c r="G18" s="42">
+      <c r="G18" s="32">
         <v>-0.31980648193264349</v>
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+    <row r="19" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
         <v>2018</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="3">
         <v>56555</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="41">
         <v>-0.53609600446227168</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="43"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="33"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+    <row r="20" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>2018</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="3">
         <v>40675</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="41">
         <v>-0.31160830639565384</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="33"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+    <row r="21" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
         <v>2018</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="14">
+      <c r="C21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="3">
         <v>86472</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="41">
         <v>-1.8846516060953333E-2</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="44"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+    <row r="22" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <v>2019</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="3">
         <v>50870</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="41">
         <v>-2.579619664094069E-2</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="29">
         <v>304475</v>
       </c>
-      <c r="G22" s="42">
+      <c r="G22" s="32">
         <v>0.2905912622552656</v>
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+    <row r="23" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>2019</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="3">
         <v>58905</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="41">
         <v>4.155247104588454E-2</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="17" t="s">
+      <c r="F23" s="30"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+    <row r="24" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
         <v>2019</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="3">
         <v>47147</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="41">
         <v>0.15911493546404426</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="33"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
+    <row r="25" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
         <v>2019</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>82</v>
+      <c r="C25" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="D25" s="3">
         <v>147553</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="41">
         <v>0.70636737903598856</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="44"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+    <row r="26" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>2020</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D26" s="3">
         <v>137220</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="41">
         <v>1.6974641242382544</v>
       </c>
-      <c r="F26" s="36">
+      <c r="F26" s="29">
         <v>1839932</v>
       </c>
-      <c r="G26" s="42">
+      <c r="G26" s="32">
         <v>5.0429657607356928</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+    <row r="27" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
         <v>2020</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="3">
         <v>100445</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="41">
         <v>0.70520329343858756</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="43"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="33"/>
       <c r="H27" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+    <row r="28" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>2020</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>74</v>
+      <c r="C28" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="D28" s="3">
         <v>61902</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="41">
         <v>0.31295734617260906</v>
       </c>
-      <c r="F28" s="37"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="33"/>
       <c r="H28" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+    <row r="29" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
         <v>2020</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>75</v>
+      <c r="C29" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="D29" s="4">
         <v>1540365</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="41">
         <v>9.4394014354164266</v>
       </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="44"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+    <row r="30" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>2021</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="4">
         <v>145868</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="41">
         <v>6.3022882961667401E-2</v>
       </c>
-      <c r="F30" s="36">
+      <c r="F30" s="29">
         <v>691564</v>
       </c>
-      <c r="G30" s="42">
+      <c r="G30" s="32">
         <v>-0.62413610937795527</v>
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+    <row r="31" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
         <v>2021</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="4">
         <v>221118</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="41">
         <v>1.2013838419035292</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="43"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="33"/>
       <c r="H31" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+    <row r="32" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>2021</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="4">
         <v>104262</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="41">
         <v>0.68430745371716584</v>
       </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="43"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="33"/>
       <c r="H32" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+    <row r="33" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>2021</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>76</v>
+      <c r="C33" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="D33" s="4">
         <v>220316</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="41">
         <v>-0.85697156193499591</v>
       </c>
-      <c r="F33" s="38"/>
-      <c r="G33" s="44"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+    <row r="34" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>2022</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="4">
         <v>173787</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="41">
         <v>0.19139907313461485</v>
       </c>
-      <c r="F34" s="36">
+      <c r="F34" s="29">
         <v>767499</v>
       </c>
-      <c r="G34" s="42">
+      <c r="G34" s="32">
         <v>0.10980184046595833</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+    <row r="35" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
         <v>2022</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="4">
         <v>112081</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="41">
         <v>-0.49311679736611219</v>
       </c>
-      <c r="F35" s="37"/>
-      <c r="G35" s="43"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="33"/>
       <c r="H35" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+    <row r="36" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
         <v>2022</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D36" s="4">
         <v>203189</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="41">
         <v>0.94883083002436175</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="33"/>
       <c r="H36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+    <row r="37" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>2022</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>77</v>
+      <c r="C37" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="D37" s="4">
         <v>278442</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="41">
         <v>0.26383013489714774</v>
       </c>
-      <c r="F37" s="38"/>
-      <c r="G37" s="44"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
+    <row r="38" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>2023</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="4">
         <v>130595</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="41">
         <v>-0.24853412510717143</v>
       </c>
-      <c r="F38" s="36">
+      <c r="F38" s="29">
         <v>1041784</v>
       </c>
-      <c r="G38" s="42">
+      <c r="G38" s="32">
         <v>0.35737505846913153</v>
       </c>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
+    <row r="39" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
         <v>2023</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="4">
         <v>107489</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E39" s="41">
         <v>-4.0970369643382909E-2</v>
       </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="43"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="33"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
+    <row r="40" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
         <v>2023</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D40" s="4">
         <v>390534</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="41">
         <v>0.92202333787754254</v>
       </c>
-      <c r="F40" s="37"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="33"/>
       <c r="H40" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
+    <row r="41" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
         <v>2023</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>78</v>
+      <c r="C41" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="D41" s="4">
         <v>413166</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="41">
         <v>0.48384941926864483</v>
       </c>
-      <c r="F41" s="38"/>
-      <c r="G41" s="44"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="34"/>
       <c r="H41" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
+    <row r="42" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
         <v>2024</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D42" s="4">
         <v>185591</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="41">
         <v>0.42111872583176996</v>
       </c>
-      <c r="F42" s="36">
+      <c r="F42" s="29">
         <v>797396</v>
       </c>
-      <c r="G42" s="42">
+      <c r="G42" s="32">
         <v>-0.23458605622662662</v>
       </c>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
+    <row r="43" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
         <v>2024</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="4">
         <v>157238</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="41">
         <v>0.46282875457023509</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="43"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="33"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10">
+    <row r="44" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
         <v>2024</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="4">
         <v>180158</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="41">
         <v>-0.53868805276877296</v>
       </c>
-      <c r="F44" s="37"/>
-      <c r="G44" s="43"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="33"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+    <row r="45" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
         <v>2024</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>79</v>
+      <c r="C45" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="D45" s="3">
         <v>274409</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="41">
         <v>-0.33583837973114922</v>
       </c>
-      <c r="F45" s="38"/>
-      <c r="G45" s="44"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="34"/>
       <c r="H45" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="48"/>
+    <row r="47" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="47" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
+    <row r="48" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
         <v>2025</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="12">
         <v>179832</v>
       </c>
-      <c r="E48" s="28">
+      <c r="E48" s="42">
         <v>-3.1030599544158929E-2</v>
       </c>
-      <c r="F48" s="30">
+      <c r="F48" s="23">
         <v>724803.4475924049</v>
       </c>
-      <c r="G48" s="33">
+      <c r="G48" s="26">
         <v>-9.1037015996562679E-2</v>
       </c>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="46">
+    <row r="49" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="21">
         <v>2025</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="18">
         <v>215752.12872392911</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="43">
         <v>0.3610494961878527</v>
       </c>
-      <c r="F49" s="31"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="22"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="16"/>
     </row>
-    <row r="50" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46">
+    <row r="50" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="21">
         <v>2025</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="18">
         <v>121531.06890325664</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="43">
         <v>0.36100002675542653</v>
       </c>
-      <c r="F50" s="31"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="22"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="16"/>
     </row>
-    <row r="51" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="46">
+    <row r="51" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="21">
         <v>2025</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="18">
+        <v>207688.24996521923</v>
+      </c>
+      <c r="E51" s="43">
+        <v>-0.18170719056843873</v>
+      </c>
+      <c r="F51" s="25"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="19"/>
+    </row>
+    <row r="52" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="44">
+        <v>2026</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="18">
+        <v>148430.38993153075</v>
+      </c>
+      <c r="E52" s="43">
+        <v>0.21185592994506547</v>
+      </c>
+      <c r="F52" s="23">
+        <v>653194.66418511141</v>
+      </c>
+      <c r="G52" s="26">
+        <v>-9.8797520410751238E-2</v>
+      </c>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="44">
+        <v>2026</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="18">
+        <v>198087.63740002186</v>
+      </c>
+      <c r="E53" s="43">
+        <v>-7.5556123975874731E-2</v>
+      </c>
+      <c r="F53" s="24"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="44">
+        <v>2026</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="18">
+        <v>122713.79697460329</v>
+      </c>
+      <c r="E54" s="43">
+        <v>-0.21318964151211378</v>
+      </c>
+      <c r="F54" s="24"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="16"/>
+    </row>
+    <row r="55" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="44">
+        <v>2026</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="24">
-        <v>207688.24996521923</v>
-      </c>
-      <c r="E51" s="25">
-        <v>-0.18170719056843873</v>
-      </c>
-      <c r="F51" s="32"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="26"/>
+      <c r="D55" s="18">
+        <v>183962.83987895545</v>
+      </c>
+      <c r="E55" s="43">
+        <v>-4.6530060564736131E-2</v>
+      </c>
+      <c r="F55" s="25"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="16"/>
     </row>
-    <row r="52" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47">
+    <row r="56" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="21">
         <v>2026</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B57" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="23" t="s">
+      <c r="C57" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="24">
-        <v>148430.38993153075</v>
-      </c>
-      <c r="E52" s="25">
-        <v>0.21185592994506547</v>
-      </c>
-      <c r="F52" s="30">
-        <v>653194.66418511141</v>
-      </c>
-      <c r="G52" s="33">
-        <v>-9.8797520410751238E-2</v>
-      </c>
-      <c r="H52" s="22"/>
+      <c r="D57" s="18">
+        <v>155665.94480820085</v>
+      </c>
+      <c r="E57" s="43">
+        <v>-0.13438128470905708</v>
+      </c>
+      <c r="F57" s="23">
+        <v>1288316.1379912619</v>
+      </c>
+      <c r="G57" s="26">
+        <v>0.97233108080956543</v>
+      </c>
+      <c r="H57" s="16"/>
     </row>
-    <row r="53" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47">
+    <row r="58" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="21">
         <v>2026</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B58" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="23" t="s">
+      <c r="C58" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="24">
-        <v>198087.63740002186</v>
-      </c>
-      <c r="E53" s="25">
-        <v>-7.5556123975874731E-2</v>
-      </c>
-      <c r="F53" s="31"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="22"/>
+      <c r="D58" s="18">
+        <v>755745.84061898128</v>
+      </c>
+      <c r="E58" s="43">
+        <v>2.502843031440094</v>
+      </c>
+      <c r="F58" s="24"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="16" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="54" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="47">
+    <row r="59" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
         <v>2026</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B59" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C59" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="24">
-        <v>122713.79697460329</v>
-      </c>
-      <c r="E54" s="25">
-        <v>-0.21318964151211378</v>
-      </c>
-      <c r="F54" s="31"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="22"/>
+      <c r="D59" s="18">
+        <v>139845.525722438</v>
+      </c>
+      <c r="E59" s="43">
+        <v>0.15069773502741254</v>
+      </c>
+      <c r="F59" s="24"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="16"/>
     </row>
-    <row r="55" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="47">
+    <row r="60" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="21">
         <v>2026</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B60" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="24">
-        <v>183962.83987895545</v>
-      </c>
-      <c r="E55" s="25">
-        <v>-4.6530060564736131E-2</v>
-      </c>
-      <c r="F55" s="32"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="22"/>
+      <c r="C60" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="18">
+        <v>237058.82684164197</v>
+      </c>
+      <c r="E60" s="43">
+        <v>0.14141665155029867</v>
+      </c>
+      <c r="F60" s="25"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="16"/>
     </row>
-    <row r="56" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="48"/>
+    <row r="61" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="57" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="47">
-        <v>2026</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" s="24">
-        <v>155665.94480820085</v>
-      </c>
-      <c r="E57" s="25">
-        <v>-0.13438128470905708</v>
-      </c>
-      <c r="F57" s="30">
-        <v>1288316.1379912619</v>
-      </c>
-      <c r="G57" s="33">
-        <v>0.97233108080956543</v>
-      </c>
-      <c r="H57" s="22"/>
+    <row r="62" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="58" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="47">
-        <v>2026</v>
-      </c>
-      <c r="B58" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" s="24">
-        <v>755745.84061898128</v>
-      </c>
-      <c r="E58" s="25">
-        <v>2.502843031440094</v>
-      </c>
-      <c r="F58" s="31"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="22" t="s">
-        <v>83</v>
+    <row r="63" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="47">
-        <v>2026</v>
-      </c>
-      <c r="B59" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="24">
-        <v>139845.52572243783</v>
-      </c>
-      <c r="E59" s="25">
-        <v>0.15069773502741254</v>
-      </c>
-      <c r="F59" s="31"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="22"/>
-    </row>
-    <row r="60" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="47">
-        <v>2026</v>
-      </c>
-      <c r="B60" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="24">
-        <v>237058.82684164197</v>
-      </c>
-      <c r="E60" s="25">
-        <v>0.14141665155029867</v>
-      </c>
-      <c r="F60" s="32"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="22"/>
-    </row>
-    <row r="61" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+    <row r="64" spans="1:8" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="29" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="G26:G29"/>
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="G38:G41"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="F38:F41"/>
     <mergeCell ref="F48:F51"/>
     <mergeCell ref="G48:G51"/>
     <mergeCell ref="F52:F55"/>
     <mergeCell ref="G52:G55"/>
     <mergeCell ref="F42:F45"/>
     <mergeCell ref="G42:G45"/>
-    <mergeCell ref="G38:G41"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="G57:G60"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>